<commit_message>
update ARIMA & SARIMA FORECASTING
</commit_message>
<xml_diff>
--- a/Datasets/COAL Consumption.xlsx
+++ b/Datasets/COAL Consumption.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KARTHIKEYA\Desktop\Mini Project\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{74416926-3981-49CD-969B-F9DCBD4CD16D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEC8E34-B30C-4AD0-83F0-4DA10D554462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{224CADB2-98E9-4EA2-8219-CFE20682AE4E}"/>
   </bookViews>
@@ -1191,7 +1191,7 @@
   <dimension ref="A1:C5522"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added Prophet to LLM's
</commit_message>
<xml_diff>
--- a/Datasets/COAL Consumption.xlsx
+++ b/Datasets/COAL Consumption.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KARTHIKEYA\Desktop\Mini Project\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49757189-510C-4B2F-BCD0-94058A355104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7153964-D8F9-41BD-B53C-225B3B6026B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{224CADB2-98E9-4EA2-8219-CFE20682AE4E}"/>
   </bookViews>
@@ -830,9 +830,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1190,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE64DB61-72FA-4E04-BB84-EDEA9783C1AB}">
   <dimension ref="A1:C5522"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1774,90 +1775,90 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="A53" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="1">
         <v>2016</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="2">
         <v>1191.6005</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="A54" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="1">
         <v>2017</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="2">
         <v>1192.7607</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="A55" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="1">
         <v>2018</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="2">
         <v>1170.1332</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+      <c r="A56" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="1">
         <v>2019</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="2">
         <v>1236.2761</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+      <c r="A57" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="1">
         <v>2020</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="2">
         <v>1195.1685</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+      <c r="A58" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="1">
         <v>2021</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="2">
         <v>1197.9290000000001</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="A59" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="1">
         <v>2022</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="2">
         <v>1144.8706999999999</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+      <c r="A60" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="1">
         <v>2023</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="2">
         <v>1133.9897000000001</v>
       </c>
     </row>

</xml_diff>